<commit_message>
Ajustes para code review
</commit_message>
<xml_diff>
--- a/diagramas_checklist/CheckListCodigo.xlsx
+++ b/diagramas_checklist/CheckListCodigo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Pablo\Desktop\Gestion_de_la_Calidad\CodeReview4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Pablo\Desktop\Gestion_de_la_Calidad\RepositorioReto\reto_frontend\diagramas_checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>CheckList Código</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Codificacion utf-8</t>
-  </si>
-  <si>
-    <t>No mezclar código CSS dentro de los archivos HTML</t>
   </si>
   <si>
     <t>Referencias de CSS al principio del HTML</t>
@@ -105,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +112,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,13 +151,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +471,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -471,7 +479,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -479,7 +487,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -487,7 +495,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -495,7 +503,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -503,7 +511,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -511,7 +519,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -519,7 +527,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -527,7 +535,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -535,7 +543,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -543,7 +551,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -551,58 +559,59 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>23</v>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
+      <c r="B16" s="2"/>
+      <c r="D16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="D17" t="s">
-        <v>23</v>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="D18" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2"/>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -610,15 +619,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>